<commit_message>
Interpretar conteúdo do Excel para gerar Nullable types #2
</commit_message>
<xml_diff>
--- a/resources/Excel.xlsx
+++ b/resources/Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sources\open-source\maestria\TypeProviders\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1A5844-F18C-431B-B82B-60DD3306CEBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59960DE-B967-41F6-8074-240263FF7F0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Id</t>
   </si>
@@ -49,13 +49,19 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Valor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +71,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -87,15 +100,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -374,27 +390,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="2" max="2" width="8.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -402,31 +422,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="3">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -434,12 +463,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version 1.0.1 Publish with Release configuration
</commit_message>
<xml_diff>
--- a/resources/Excel.xlsx
+++ b/resources/Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sources\open-source\maestria\TypeProviders\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F313B76-0032-4CD0-8159-D1B3F9338394}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91FAAB6-B0C5-4EC6-A38E-81E0BCD35459}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Id</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>Birth Date</t>
+  </si>
+  <si>
+    <t>Nova Propriedade</t>
   </si>
 </sst>
 </file>
@@ -394,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,9 +409,10 @@
     <col min="2" max="2" width="8.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="3"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -421,8 +425,11 @@
       <c r="D1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -432,8 +439,11 @@
       <c r="D2" s="4">
         <v>31840</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -446,8 +456,11 @@
       <c r="D3" s="4">
         <v>31841</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -460,8 +473,11 @@
       <c r="D4" s="4">
         <v>31842</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -474,8 +490,11 @@
       <c r="D5" s="4">
         <v>31843</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -485,8 +504,11 @@
       <c r="D6" s="4">
         <v>31844</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -498,6 +520,9 @@
       </c>
       <c r="D7" s="4">
         <v>31845</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Load page position support
</commit_message>
<xml_diff>
--- a/resources/Excel.xlsx
+++ b/resources/Excel.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sources\open-source\maestria\TypeProviders\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A665256-68B4-427E-9C51-03E0E047D669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEB5D7E-AE75-46DB-8468-82F9DF359494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3210" yWindow="2325" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
   <si>
     <t>Id</t>
   </si>
@@ -412,7 +413,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,4 +570,188 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F68805-6DFE-4FE4-8F49-4D8BA4B65A85}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>31840</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <f>E2+10</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4">
+        <v>31841</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F7" si="0">E3+10</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>5.01</v>
+      </c>
+      <c r="D4" s="4">
+        <v>31842</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4">
+        <v>31843</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>31844</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3">
+        <v>9</v>
+      </c>
+      <c r="D7" s="4">
+        <v>31845</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3">
+        <v>9</v>
+      </c>
+      <c r="D8" s="4">
+        <v>31845</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ref="F8" si="1">E8+10</f>
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
1.0.7 Sheet support excel file
</commit_message>
<xml_diff>
--- a/resources/Excel.xlsx
+++ b/resources/Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sources\open-source\maestria\TypeProviders\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEB5D7E-AE75-46DB-8468-82F9DF359494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B375C192-4F80-4237-B771-65F3787B6345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3210" yWindow="2325" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Id</t>
   </si>
@@ -71,6 +71,30 @@
   </si>
   <si>
     <t>Calculated Prop</t>
+  </si>
+  <si>
+    <t>Prop Sheet 2</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -574,10 +598,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99F68805-6DFE-4FE4-8F49-4D8BA4B65A85}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,9 +612,10 @@
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,8 +634,11 @@
       <c r="F1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -627,8 +655,11 @@
         <f>E2+10</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -648,8 +679,11 @@
         <f t="shared" ref="F3:F7" si="0">E3+10</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -669,8 +703,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -690,8 +727,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -708,8 +748,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -729,8 +772,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -749,6 +795,9 @@
       <c r="F8">
         <f t="shared" ref="F8" si="1">E8+10</f>
         <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bugfix: remove special char to generate dotnet property name
</commit_message>
<xml_diff>
--- a/resources/Excel.xlsx
+++ b/resources/Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sources\open-source\maestria\TypeProviders\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B375C192-4F80-4237-B771-65F3787B6345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6573B7-F9B9-463C-B135-257B11905E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="2325" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="27">
   <si>
     <t>Id</t>
   </si>
@@ -95,6 +95,27 @@
   </si>
   <si>
     <t>g</t>
+  </si>
+  <si>
+    <t>Prop sample</t>
+  </si>
+  <si>
+    <t>Prop  \  sample  /  a   b</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>Prop-sample 2</t>
+  </si>
+  <si>
+    <t>Prop_sample 3</t>
+  </si>
+  <si>
+    <t>Prop\sample 4</t>
+  </si>
+  <si>
+    <t>Prop/sample 5</t>
   </si>
 </sst>
 </file>
@@ -434,23 +455,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -469,8 +496,26 @@
       <c r="F1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -487,8 +532,26 @@
         <f>E2+10</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -508,8 +571,26 @@
         <f t="shared" ref="F3:F7" si="0">E3+10</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -529,8 +610,26 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -550,8 +649,26 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -568,8 +685,26 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -588,6 +723,24 @@
       <c r="F7">
         <f t="shared" si="0"/>
         <v>16</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>